<commit_message>
#4801_PreRegister Module: payment_export (Restart & Update Module) https://mobileapp.nstda.or.th/redmine/issues/4801
</commit_message>
<xml_diff>
--- a/payment_export/export_template/xlsx_report_register_icash_direct.xlsx
+++ b/payment_export/export_template/xlsx_report_register_icash_direct.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Pre Register iCash</t>
   </si>
@@ -49,6 +49,9 @@
   </si>
   <si>
     <t>Bene Email Address</t>
+  </si>
+  <si>
+    <t>Run Date</t>
   </si>
 </sst>
 </file>
@@ -89,7 +92,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -114,6 +117,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="7">
     <border>
@@ -210,7 +219,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -249,6 +258,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -256,6 +269,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF99"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -533,7 +551,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
@@ -567,6 +587,12 @@
       <c r="D2" s="10"/>
       <c r="E2" s="7"/>
     </row>
+    <row r="3" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="15"/>
+    </row>
     <row r="5" spans="1:8" s="13" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>5</v>

</xml_diff>